<commit_message>
se modifica archivo plantilla y se cambia consulta de validación de el proceso, ya que el umero de proceso se puede repetir
</commit_message>
<xml_diff>
--- a/public/archivos/archivoexcel.xlsx
+++ b/public/archivos/archivoexcel.xlsx
@@ -1503,15 +1503,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1539,13 +1539,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G979" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I997" activeCellId="0" sqref="I997"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27"/>
@@ -1589,7 +1589,7 @@
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
         <v>1</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>2</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
         <v>3</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>4</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
         <v>5</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
         <v>6</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
         <v>7</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
         <v>8</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
         <v>9</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
         <v>10</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
         <v>11</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
         <v>12</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>13</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
         <v>14</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
         <v>15</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
         <v>16</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
         <v>17</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
         <v>18</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
         <v>19</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
         <v>20</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
         <v>21</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
         <v>22</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
         <v>23</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
         <v>24</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
         <v>25</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="n">
         <v>26</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="n">
         <v>27</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
         <v>28</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
         <v>29</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
         <v>30</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
         <v>31</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
         <v>32</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
         <v>33</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="n">
         <v>34</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
         <v>35</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
         <v>36</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
         <v>37</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="231" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
         <v>38</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
         <v>39</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
         <v>40</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="n">
         <v>41</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="n">
         <v>42</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="n">
         <v>43</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="n">
         <v>44</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="n">
         <v>45</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
         <v>46</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
         <v>47</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
         <v>48</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="n">
         <v>49</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="n">
         <v>50</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="n">
         <v>51</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="n">
         <v>52</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="n">
         <v>53</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="n">
         <v>54</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="n">
         <v>55</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="n">
         <v>56</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="n">
         <v>57</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="n">
         <v>58</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="n">
         <v>59</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="n">
         <v>60</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="n">
         <v>61</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="n">
         <v>62</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="n">
         <v>63</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="n">
         <v>64</v>
       </c>
@@ -3445,7 +3445,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="n">
         <v>65</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="163.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="n">
         <v>66</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="n">
         <v>67</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="n">
         <v>68</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="n">
         <v>69</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="n">
         <v>70</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="n">
         <v>71</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="n">
         <v>72</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="n">
         <v>73</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="n">
         <v>74</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="n">
         <v>75</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="n">
         <v>76</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="n">
         <v>77</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="n">
         <v>78</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="n">
         <v>79</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="163.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="n">
         <v>80</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="n">
         <v>81</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="n">
         <v>82</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="n">
         <v>83</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="n">
         <v>84</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="n">
         <v>85</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="123" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="n">
         <v>86</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="217.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="216.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="n">
         <v>87</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="n">
         <v>88</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="n">
         <v>89</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="n">
         <v>90</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6" t="n">
         <v>91</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="n">
         <v>92</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="150" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="n">
         <v>93</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="n">
         <v>94</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="312" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="n">
         <v>95</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="96" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="n">
         <v>96</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="189.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="n">
         <v>97</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="204" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="n">
         <v>98</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="109.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="n">
         <v>99</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="n">
         <v>100</v>
       </c>
@@ -10773,106 +10773,106 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="MÍNIMA CUANTÍA HIL-CEFA-0004-2019 "/>
-    <hyperlink ref="B3" r:id="rId2" display="SG-MC-24 "/>
-    <hyperlink ref="B4" r:id="rId3" display="INVITACION 018-2019 "/>
-    <hyperlink ref="B5" r:id="rId4" display="SAM 02 - 2019 "/>
-    <hyperlink ref="B6" r:id="rId5" display="CMI-033-2019 "/>
-    <hyperlink ref="B7" r:id="rId6" display="CAL-MC-001-2019 "/>
-    <hyperlink ref="B8" r:id="rId7" display="IPMC #005 DE 2019 "/>
-    <hyperlink ref="B9" r:id="rId8" display="SD-016-2019 "/>
-    <hyperlink ref="B10" r:id="rId9" display="CMC 022-2019 "/>
-    <hyperlink ref="B11" r:id="rId10" display="MC-CS-015-2019 "/>
-    <hyperlink ref="B12" r:id="rId11" display="CMC 021-2019 "/>
-    <hyperlink ref="B13" r:id="rId12" display="MC 041-2019 "/>
-    <hyperlink ref="B14" r:id="rId13" display="MC 040-2019 "/>
-    <hyperlink ref="B15" r:id="rId14" display="CMC 020-2019 "/>
-    <hyperlink ref="B16" r:id="rId15" display="MC 038-2019 "/>
-    <hyperlink ref="B17" r:id="rId16" display="MC 039-2019 "/>
-    <hyperlink ref="B18" r:id="rId17" display="CMC 019-2019 "/>
-    <hyperlink ref="B19" r:id="rId18" display="IPMC-038-2019 "/>
-    <hyperlink ref="B20" r:id="rId19" display="CMIC-024-2019 "/>
-    <hyperlink ref="B21" r:id="rId20" display="IPMC-ALGE No. 018 DE 2019 "/>
-    <hyperlink ref="B22" r:id="rId21" display="MC-016-2019 "/>
-    <hyperlink ref="B23" r:id="rId22" display="IPMC.040-2019 "/>
-    <hyperlink ref="B24" r:id="rId23" display="IPMC-NATA 021 DE 2019 "/>
-    <hyperlink ref="B25" r:id="rId24" display="MC-MZ-041-2019 "/>
-    <hyperlink ref="B26" r:id="rId25" display="MINIMA CUANTIA 012-2019 "/>
-    <hyperlink ref="B27" r:id="rId26" display="MC-015-2019 "/>
-    <hyperlink ref="B28" r:id="rId27" display="OGAD-CPS-099-2019 "/>
-    <hyperlink ref="B29" r:id="rId28" display="MC-026-2019 "/>
-    <hyperlink ref="B30" r:id="rId29" display="PSMC-014-LSC-2019 "/>
-    <hyperlink ref="B31" r:id="rId30" display="INVITACION SP-005-2019 "/>
-    <hyperlink ref="B32" r:id="rId31" display="AMBC-MC-014-2019 "/>
-    <hyperlink ref="B33" r:id="rId32" display="MP MC 003 DE 2019 "/>
-    <hyperlink ref="B34" r:id="rId33" display="SMC-050-2019 "/>
-    <hyperlink ref="B35" r:id="rId34" display="MC-015-2019 "/>
-    <hyperlink ref="B36" r:id="rId35" display="C.M.C No. 016 DE 2019 "/>
-    <hyperlink ref="B37" r:id="rId36" display="MC-027-19 "/>
-    <hyperlink ref="B38" r:id="rId37" display="PSMC-012-LSC-2019 "/>
-    <hyperlink ref="B39" r:id="rId38" display="INVITACION PUBLICA DE MINIMA CUANTIA 07 - 2019 "/>
-    <hyperlink ref="B40" r:id="rId39" display="2019-000-026 "/>
-    <hyperlink ref="B41" r:id="rId40" display="001 del 2019 "/>
-    <hyperlink ref="B42" r:id="rId41" display="162-2019 "/>
-    <hyperlink ref="B43" r:id="rId42" display="163-2019 "/>
-    <hyperlink ref="B44" r:id="rId43" display="IP-2019-STTM-010 "/>
-    <hyperlink ref="B45" r:id="rId44" display="MIN 014 DE 2019 "/>
-    <hyperlink ref="B46" r:id="rId45" display="PSMC-013-LSC-2019 "/>
-    <hyperlink ref="B47" r:id="rId46" display="LB MC - 011 de 2019 "/>
-    <hyperlink ref="B48" r:id="rId47" display="SPDM-C0-098-2019 "/>
-    <hyperlink ref="B49" r:id="rId48" display="386 "/>
-    <hyperlink ref="B50" r:id="rId49" display="MC. 035-2019 "/>
-    <hyperlink ref="B51" r:id="rId50" display="MC-014-2019 "/>
-    <hyperlink ref="B52" r:id="rId51" display="MC. 034-2019 "/>
-    <hyperlink ref="B53" r:id="rId52" display="IPMC-NATA 020 DE 2019 "/>
-    <hyperlink ref="B54" r:id="rId53" display="041-2019 "/>
-    <hyperlink ref="B55" r:id="rId54" display="MC-019-11/04/2019 "/>
-    <hyperlink ref="B56" r:id="rId55" display="CHAMEZA-MC-061-2019 "/>
-    <hyperlink ref="B57" r:id="rId56" display="CMC 030 DE 2019 "/>
-    <hyperlink ref="B58" r:id="rId57" display="CMC 028 DE 2019 "/>
-    <hyperlink ref="B59" r:id="rId58" display="CMC 029 DE 2019 "/>
-    <hyperlink ref="B60" r:id="rId59" display="IP.021.2019 "/>
-    <hyperlink ref="B61" r:id="rId60" display="IMC 024-2019 "/>
-    <hyperlink ref="B62" r:id="rId61" display="MC-009-2019 "/>
-    <hyperlink ref="B63" r:id="rId62" display="MC-028-2018 "/>
-    <hyperlink ref="B64" r:id="rId63" display="INV-008-2019 "/>
-    <hyperlink ref="B65" r:id="rId64" display="MINC-MG 025-2019 "/>
-    <hyperlink ref="B66" r:id="rId65" display="DC-SDEC-MC-40-2019 "/>
-    <hyperlink ref="B67" r:id="rId66" display="MC-019-2019 "/>
-    <hyperlink ref="B68" r:id="rId67" display="INV-007-2019 "/>
-    <hyperlink ref="B69" r:id="rId68" display="MC-014-2019 "/>
-    <hyperlink ref="B70" r:id="rId69" display="023-2019 "/>
-    <hyperlink ref="B71" r:id="rId70" display="MGMC 012 "/>
-    <hyperlink ref="B72" r:id="rId71" display="NDS-CIES-0217-2019 "/>
-    <hyperlink ref="B73" r:id="rId72" display="MC 026 DE 2019 "/>
-    <hyperlink ref="B74" r:id="rId73" display="DC-SG- MC-36-2019 "/>
-    <hyperlink ref="B75" r:id="rId74" display="MC-057-2019 "/>
-    <hyperlink ref="B76" r:id="rId75" display="MDT-PSMIC-029-2019 "/>
-    <hyperlink ref="B77" r:id="rId76" display="MVC-SMINC-012-2019 "/>
-    <hyperlink ref="B78" r:id="rId77" display="SMC-018-2019 "/>
-    <hyperlink ref="B79" r:id="rId78" display="SMC-019-2019 "/>
-    <hyperlink ref="B80" r:id="rId79" display="MIC-009-2019 "/>
-    <hyperlink ref="B81" r:id="rId80" display="MC 022-2019 "/>
-    <hyperlink ref="B82" r:id="rId81" display="MC 023-2019 "/>
-    <hyperlink ref="B83" r:id="rId82" display="MC-SMC-038-2019 "/>
-    <hyperlink ref="B84" r:id="rId83" display="MC-SMC-037-2019 "/>
-    <hyperlink ref="B85" r:id="rId84" display="MC-SMC-039-2019 "/>
-    <hyperlink ref="B86" r:id="rId85" display="S-MC-MZ-035-2019 "/>
-    <hyperlink ref="B87" r:id="rId86" display="INVI-012 "/>
-    <hyperlink ref="B88" r:id="rId87" display="MC-SEG-025-2019 "/>
-    <hyperlink ref="B89" r:id="rId88" display="S-MC-MZ-036-2019 "/>
-    <hyperlink ref="B90" r:id="rId89" display="PSmc-PL-014-2019 "/>
-    <hyperlink ref="B91" r:id="rId90" display="0272019 "/>
-    <hyperlink ref="B92" r:id="rId91" display="MC-2019000575 "/>
-    <hyperlink ref="B93" r:id="rId92" display="MC - 010 - 2019 "/>
-    <hyperlink ref="B94" r:id="rId93" display="PSmc-G-044-2019 "/>
-    <hyperlink ref="B95" r:id="rId94" display="mc 002 2019 "/>
-    <hyperlink ref="B96" r:id="rId95" display="MIC IP-015-2019 "/>
-    <hyperlink ref="B97" r:id="rId96" display="MC 057 DE 2019 "/>
-    <hyperlink ref="B98" r:id="rId97" display="MC-SICC-06-2019 "/>
-    <hyperlink ref="B99" r:id="rId98" display="IP-2019-032 "/>
-    <hyperlink ref="B100" r:id="rId99" display="SUMINISTRO INV 039 11/04/2019 "/>
-    <hyperlink ref="B101" r:id="rId100" display="M-CMS-008-2019 "/>
+    <hyperlink ref="B2" r:id="rId1" display="MÍNIMA CUANTÍA HIL-CEFA-0004-2019"/>
+    <hyperlink ref="B3" r:id="rId2" display="SG-MC-24"/>
+    <hyperlink ref="B4" r:id="rId3" display="INVITACION 018-2019"/>
+    <hyperlink ref="B5" r:id="rId4" display="SAM 02 - 2019"/>
+    <hyperlink ref="B6" r:id="rId5" display="CMI-033-2019"/>
+    <hyperlink ref="B7" r:id="rId6" display="CAL-MC-001-2019"/>
+    <hyperlink ref="B8" r:id="rId7" display="IPMC #005 DE 2019"/>
+    <hyperlink ref="B9" r:id="rId8" display="SD-016-2019"/>
+    <hyperlink ref="B10" r:id="rId9" display="CMC 022-2019"/>
+    <hyperlink ref="B11" r:id="rId10" display="MC-CS-015-2019"/>
+    <hyperlink ref="B12" r:id="rId11" display="CMC 021-2019"/>
+    <hyperlink ref="B13" r:id="rId12" display="MC 041-2019"/>
+    <hyperlink ref="B14" r:id="rId13" display="MC 040-2019"/>
+    <hyperlink ref="B15" r:id="rId14" display="CMC 020-2019"/>
+    <hyperlink ref="B16" r:id="rId15" display="MC 038-2019"/>
+    <hyperlink ref="B17" r:id="rId16" display="MC 039-2019"/>
+    <hyperlink ref="B18" r:id="rId17" display="CMC 019-2019"/>
+    <hyperlink ref="B19" r:id="rId18" display="IPMC-038-2019"/>
+    <hyperlink ref="B20" r:id="rId19" display="CMIC-024-2019"/>
+    <hyperlink ref="B21" r:id="rId20" display="IPMC-ALGE No. 018 DE 2019"/>
+    <hyperlink ref="B22" r:id="rId21" display="MC-016-2019"/>
+    <hyperlink ref="B23" r:id="rId22" display="IPMC.040-2019"/>
+    <hyperlink ref="B24" r:id="rId23" display="IPMC-NATA 021 DE 2019"/>
+    <hyperlink ref="B25" r:id="rId24" display="MC-MZ-041-2019"/>
+    <hyperlink ref="B26" r:id="rId25" display="MINIMA CUANTIA 012-2019"/>
+    <hyperlink ref="B27" r:id="rId26" display="MC-015-2019"/>
+    <hyperlink ref="B28" r:id="rId27" display="OGAD-CPS-099-2019"/>
+    <hyperlink ref="B29" r:id="rId28" display="MC-026-2019"/>
+    <hyperlink ref="B30" r:id="rId29" display="PSMC-014-LSC-2019"/>
+    <hyperlink ref="B31" r:id="rId30" display="INVITACION SP-005-2019"/>
+    <hyperlink ref="B32" r:id="rId31" display="AMBC-MC-014-2019"/>
+    <hyperlink ref="B33" r:id="rId32" display="MP MC 003 DE 2019"/>
+    <hyperlink ref="B34" r:id="rId33" display="SMC-050-2019"/>
+    <hyperlink ref="B35" r:id="rId34" display="MC-015-2019"/>
+    <hyperlink ref="B36" r:id="rId35" display="C.M.C No. 016 DE 2019"/>
+    <hyperlink ref="B37" r:id="rId36" display="MC-027-19"/>
+    <hyperlink ref="B38" r:id="rId37" display="PSMC-012-LSC-2019"/>
+    <hyperlink ref="B39" r:id="rId38" display="INVITACION PUBLICA DE MINIMA CUANTIA 07 - 2019"/>
+    <hyperlink ref="B40" r:id="rId39" display="2019-000-026"/>
+    <hyperlink ref="B41" r:id="rId40" display="001 del 2019"/>
+    <hyperlink ref="B42" r:id="rId41" display="162-2019"/>
+    <hyperlink ref="B43" r:id="rId42" display="163-2019"/>
+    <hyperlink ref="B44" r:id="rId43" display="IP-2019-STTM-010"/>
+    <hyperlink ref="B45" r:id="rId44" display="MIN 014 DE 2019"/>
+    <hyperlink ref="B46" r:id="rId45" display="PSMC-013-LSC-2019"/>
+    <hyperlink ref="B47" r:id="rId46" display="LB MC - 011 de 2019"/>
+    <hyperlink ref="B48" r:id="rId47" display="SPDM-C0-098-2019"/>
+    <hyperlink ref="B49" r:id="rId48" display="386"/>
+    <hyperlink ref="B50" r:id="rId49" display="MC. 035-2019"/>
+    <hyperlink ref="B51" r:id="rId50" display="MC-014-2019"/>
+    <hyperlink ref="B52" r:id="rId51" display="MC. 034-2019"/>
+    <hyperlink ref="B53" r:id="rId52" display="IPMC-NATA 020 DE 2019"/>
+    <hyperlink ref="B54" r:id="rId53" display="041-2019"/>
+    <hyperlink ref="B55" r:id="rId54" display="MC-019-11/04/2019"/>
+    <hyperlink ref="B56" r:id="rId55" display="CHAMEZA-MC-061-2019"/>
+    <hyperlink ref="B57" r:id="rId56" display="CMC 030 DE 2019"/>
+    <hyperlink ref="B58" r:id="rId57" display="CMC 028 DE 2019"/>
+    <hyperlink ref="B59" r:id="rId58" display="CMC 029 DE 2019"/>
+    <hyperlink ref="B60" r:id="rId59" display="IP.021.2019"/>
+    <hyperlink ref="B61" r:id="rId60" display="IMC 024-2019"/>
+    <hyperlink ref="B62" r:id="rId61" display="MC-009-2019"/>
+    <hyperlink ref="B63" r:id="rId62" display="MC-028-2018"/>
+    <hyperlink ref="B64" r:id="rId63" display="INV-008-2019"/>
+    <hyperlink ref="B65" r:id="rId64" display="MINC-MG 025-2019"/>
+    <hyperlink ref="B66" r:id="rId65" display="DC-SDEC-MC-40-2019"/>
+    <hyperlink ref="B67" r:id="rId66" display="MC-019-2019"/>
+    <hyperlink ref="B68" r:id="rId67" display="INV-007-2019"/>
+    <hyperlink ref="B69" r:id="rId68" display="MC-014-2019"/>
+    <hyperlink ref="B70" r:id="rId69" display="023-2019"/>
+    <hyperlink ref="B71" r:id="rId70" display="MGMC 012"/>
+    <hyperlink ref="B72" r:id="rId71" display="NDS-CIES-0217-2019"/>
+    <hyperlink ref="B73" r:id="rId72" display="MC 026 DE 2019"/>
+    <hyperlink ref="B74" r:id="rId73" display="DC-SG- MC-36-2019"/>
+    <hyperlink ref="B75" r:id="rId74" display="MC-057-2019"/>
+    <hyperlink ref="B76" r:id="rId75" display="MDT-PSMIC-029-2019"/>
+    <hyperlink ref="B77" r:id="rId76" display="MVC-SMINC-012-2019"/>
+    <hyperlink ref="B78" r:id="rId77" display="SMC-018-2019"/>
+    <hyperlink ref="B79" r:id="rId78" display="SMC-019-2019"/>
+    <hyperlink ref="B80" r:id="rId79" display="MIC-009-2019"/>
+    <hyperlink ref="B81" r:id="rId80" display="MC 022-2019"/>
+    <hyperlink ref="B82" r:id="rId81" display="MC 023-2019"/>
+    <hyperlink ref="B83" r:id="rId82" display="MC-SMC-038-2019"/>
+    <hyperlink ref="B84" r:id="rId83" display="MC-SMC-037-2019"/>
+    <hyperlink ref="B85" r:id="rId84" display="MC-SMC-039-2019"/>
+    <hyperlink ref="B86" r:id="rId85" display="S-MC-MZ-035-2019"/>
+    <hyperlink ref="B87" r:id="rId86" display="INVI-012"/>
+    <hyperlink ref="B88" r:id="rId87" display="MC-SEG-025-2019"/>
+    <hyperlink ref="B89" r:id="rId88" display="S-MC-MZ-036-2019"/>
+    <hyperlink ref="B90" r:id="rId89" display="PSmc-PL-014-2019"/>
+    <hyperlink ref="B91" r:id="rId90" display="0272019"/>
+    <hyperlink ref="B92" r:id="rId91" display="MC-2019000575"/>
+    <hyperlink ref="B93" r:id="rId92" display="MC - 010 - 2019"/>
+    <hyperlink ref="B94" r:id="rId93" display="PSmc-G-044-2019"/>
+    <hyperlink ref="B95" r:id="rId94" display="mc 002 2019"/>
+    <hyperlink ref="B96" r:id="rId95" display="MIC IP-015-2019"/>
+    <hyperlink ref="B97" r:id="rId96" display="MC 057 DE 2019"/>
+    <hyperlink ref="B98" r:id="rId97" display="MC-SICC-06-2019"/>
+    <hyperlink ref="B99" r:id="rId98" display="IP-2019-032"/>
+    <hyperlink ref="B100" r:id="rId99" display="SUMINISTRO INV 039 11/04/2019"/>
+    <hyperlink ref="B101" r:id="rId100" display="M-CMS-008-2019"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>